<commit_message>
junits for all but 3 control characters
all but 3 sanskrit99 characters have unit tests
</commit_message>
<xml_diff>
--- a/notes/Sanskrit99_Conversion_Mapping.xlsx
+++ b/notes/Sanskrit99_Conversion_Mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
@@ -7295,8 +7295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9957,7 +9957,7 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98">
-        <f t="shared" ref="A98:A129" si="9">HEX2DEC(MID(B98,3,4))</f>
+        <f t="shared" ref="A98:A121" si="9">HEX2DEC(MID(B98,3,4))</f>
         <v>159</v>
       </c>
       <c r="B98" t="s">
@@ -9996,7 +9996,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x9c</v>
       </c>
-      <c r="I99" s="14" t="str">
+      <c r="I99" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_156() throws Exception { verify( (char) 156, ""); }</v>
       </c>
@@ -10042,7 +10042,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x9a</v>
       </c>
-      <c r="I101" s="14" t="str">
+      <c r="I101" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_154() throws Exception { verify( (char) 154, ""); }</v>
       </c>
@@ -10065,7 +10065,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x99</v>
       </c>
-      <c r="I102" s="14" t="str">
+      <c r="I102" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_153() throws Exception { verify( (char) 153, ""); }</v>
       </c>
@@ -10088,7 +10088,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x98</v>
       </c>
-      <c r="I103" s="14" t="str">
+      <c r="I103" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_152() throws Exception { verify( (char) 152, ""); }</v>
       </c>
@@ -10111,7 +10111,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x97</v>
       </c>
-      <c r="I104" s="14" t="str">
+      <c r="I104" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_151() throws Exception { verify( (char) 151, ""); }</v>
       </c>
@@ -10134,7 +10134,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x96</v>
       </c>
-      <c r="I105" s="14" t="str">
+      <c r="I105" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_150() throws Exception { verify( (char) 150, ""); }</v>
       </c>
@@ -10180,7 +10180,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x94</v>
       </c>
-      <c r="I107" s="14" t="str">
+      <c r="I107" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_148() throws Exception { verify( (char) 148, ""); }</v>
       </c>
@@ -10203,7 +10203,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x93</v>
       </c>
-      <c r="I108" s="14" t="str">
+      <c r="I108" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_147() throws Exception { verify( (char) 147, ""); }</v>
       </c>
@@ -10226,7 +10226,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x92</v>
       </c>
-      <c r="I109" s="14" t="str">
+      <c r="I109" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_146() throws Exception { verify( (char) 146, ""); }</v>
       </c>
@@ -10252,7 +10252,7 @@
         <v>\xc2\x91</v>
       </c>
       <c r="H110"/>
-      <c r="I110" s="14" t="str">
+      <c r="I110" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_145() throws Exception { verify( (char) 145, ""); }</v>
       </c>
@@ -10278,7 +10278,7 @@
         <v>\xc2\x8c</v>
       </c>
       <c r="H111"/>
-      <c r="I111" s="14" t="str">
+      <c r="I111" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_140() throws Exception { verify( (char) 140, ""); }</v>
       </c>
@@ -10301,7 +10301,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x8b</v>
       </c>
-      <c r="I112" s="14" t="str">
+      <c r="I112" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_139() throws Exception { verify( (char) 139, ""); }</v>
       </c>
@@ -10324,7 +10324,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x8a</v>
       </c>
-      <c r="I113" s="14" t="str">
+      <c r="I113" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_138() throws Exception { verify( (char) 138, ""); }</v>
       </c>
@@ -10347,7 +10347,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x89</v>
       </c>
-      <c r="I114" s="14" t="str">
+      <c r="I114" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_137() throws Exception { verify( (char) 137, ""); }</v>
       </c>
@@ -10370,7 +10370,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x88</v>
       </c>
-      <c r="I115" s="14" t="str">
+      <c r="I115" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_136() throws Exception { verify( (char) 136, ""); }</v>
       </c>
@@ -10416,7 +10416,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x86</v>
       </c>
-      <c r="I117" s="14" t="str">
+      <c r="I117" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_134() throws Exception { verify( (char) 134, ""); }</v>
       </c>
@@ -10439,7 +10439,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x85</v>
       </c>
-      <c r="I118" s="14" t="str">
+      <c r="I118" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_133() throws Exception { verify( (char) 133, ""); }</v>
       </c>
@@ -10462,7 +10462,7 @@
         <f t="shared" si="10"/>
         <v>\xc2\x84</v>
       </c>
-      <c r="I119" s="14" t="str">
+      <c r="I119" s="25" t="str">
         <f t="shared" si="11"/>
         <v>@Test public void testConvert_132() throws Exception { verify( (char) 132, ""); }</v>
       </c>
@@ -12203,7 +12203,7 @@
     </row>
     <row r="189" spans="1:9">
       <c r="A189">
-        <f t="shared" ref="A189:A220" si="18">HEX2DEC(MID(B189,3,4))</f>
+        <f t="shared" ref="A189:A202" si="18">HEX2DEC(MID(B189,3,4))</f>
         <v>62</v>
       </c>
       <c r="B189" t="s">

</xml_diff>